<commit_message>
Creation of the menu and the ability to create your own file
</commit_message>
<xml_diff>
--- a/my_cryptos.xlsx
+++ b/my_cryptos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\Documents\Projetcs Python\CryptoUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BB8F3B-5F72-4687-A848-45571495DD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3973EF2E-2B2B-4439-9162-E2BABC97D2A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed the gitignore and modified the menu
</commit_message>
<xml_diff>
--- a/my_cryptos.xlsx
+++ b/my_cryptos.xlsx
@@ -1,105 +1,52 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\Documents\Projetcs Python\CryptoUpdate\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3973EF2E-2B2B-4439-9162-E2BABC97D2A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
-  <si>
-    <t>CRYPTOS</t>
-  </si>
-  <si>
-    <t>BUY IN PRICE</t>
-  </si>
-  <si>
-    <t>NUMBER OF COINS</t>
-  </si>
-  <si>
-    <t>VALUE</t>
-  </si>
-  <si>
-    <t>SEI</t>
-  </si>
-  <si>
-    <t>0.0%</t>
-  </si>
-  <si>
-    <t>SHIB</t>
-  </si>
-  <si>
-    <t>XRP</t>
-  </si>
-  <si>
-    <t>PEPE</t>
-  </si>
-  <si>
-    <t>-0.13055%</t>
-  </si>
-  <si>
-    <t>BOME</t>
-  </si>
-  <si>
-    <t>FET</t>
-  </si>
-  <si>
-    <t>0.05058%</t>
-  </si>
-  <si>
-    <t>GAIN/LOSSES (ROUNDED)</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -117,33 +64,93 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -463,146 +470,205 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col width="16.7109375" customWidth="1" min="1" max="1"/>
+    <col width="15.85546875" customWidth="1" min="2" max="2"/>
+    <col width="20.5703125" customWidth="1" min="3" max="3"/>
+    <col width="21.5703125" customWidth="1" min="4" max="4"/>
+    <col width="25.5703125" customWidth="1" min="5" max="5"/>
+    <col width="20.42578125" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="3">
-        <v>21.02</v>
-      </c>
-      <c r="C2">
-        <v>27.4</v>
-      </c>
-      <c r="D2">
-        <v>21.02</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3">
-        <v>19.920000000000002</v>
-      </c>
-      <c r="C3">
-        <v>704633.89</v>
-      </c>
-      <c r="D3">
-        <v>19.920000000000002</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="3">
-        <v>42.84</v>
-      </c>
-      <c r="C4">
-        <v>71.09</v>
-      </c>
-      <c r="D4">
-        <v>42.84</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="3">
-        <v>15.32</v>
-      </c>
-      <c r="C5">
-        <v>1989610.39</v>
-      </c>
-      <c r="D5">
-        <v>15.3</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3">
-        <v>1.9</v>
-      </c>
-      <c r="C6">
-        <v>111.69</v>
-      </c>
-      <c r="D6">
-        <v>1.9</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="3">
-        <v>19.77</v>
-      </c>
-      <c r="C7">
-        <v>6.89</v>
-      </c>
-      <c r="D7">
-        <v>19.78</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>12</v>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>CRYPTOS</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>BUY IN PRICE</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>NUMBER OF COINS</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>VALUE</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>GAIN/LOSSES (ROUNDED)</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="n"/>
+      <c r="G1" s="4" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>STX</t>
+        </is>
+      </c>
+      <c r="B2" s="6" t="n">
+        <v>20.71</v>
+      </c>
+      <c r="C2" t="n">
+        <v>6.56</v>
+      </c>
+      <c r="D2" t="n">
+        <v>20.71</v>
+      </c>
+      <c r="E2" s="5" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>XRP</t>
+        </is>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>18.1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>30.78</v>
+      </c>
+      <c r="D3" t="n">
+        <v>18.1</v>
+      </c>
+      <c r="E3" s="5" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>RNDR</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>17.84</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.89</v>
+      </c>
+      <c r="D4" t="n">
+        <v>17.85</v>
+      </c>
+      <c r="E4" s="5" t="inlineStr">
+        <is>
+          <t>0.05605%</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>SEI</t>
+        </is>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>17.8</v>
+      </c>
+      <c r="C5" t="n">
+        <v>25.05</v>
+      </c>
+      <c r="D5" t="n">
+        <v>17.8</v>
+      </c>
+      <c r="E5" s="5" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>FET</t>
+        </is>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>16.99</v>
+      </c>
+      <c r="C6" t="n">
+        <v>6.51</v>
+      </c>
+      <c r="D6" t="n">
+        <v>16.99</v>
+      </c>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>UNI</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="n">
+        <v>12.26</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="D7" t="n">
+        <v>12.24</v>
+      </c>
+      <c r="E7" s="5" t="inlineStr">
+        <is>
+          <t>-0.16313%</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>LINK</t>
+        </is>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>-3.2967%</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>